<commit_message>
switch col name and SID
</commit_message>
<xml_diff>
--- a/TA/InputGrades.xlsx
+++ b/TA/InputGrades.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Yes</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Q2</t>
+  </si>
+  <si>
+    <t>Hello WORLD</t>
   </si>
 </sst>
 </file>
@@ -203,6 +206,16 @@
   <dxfs count="5">
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -218,16 +231,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -529,16 +532,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
     <col min="6" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
@@ -552,11 +555,11 @@
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E1" s="1" t="str">
         <f>IF(ISBLANK(Output!E1), "", Output!E1)</f>
@@ -653,14 +656,14 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <f>IF(ISBLANK(Input!D2), Input!C2 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D2,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C2), Input!D2 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C2,Name2SID!D:D,0)))</f>
         <v>1155000001</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A2,Name2SID!A:A,0))</f>
         <v>David HILBERT</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="1">
@@ -672,14 +675,14 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <f>IF(ISBLANK(Input!D3), Input!C3 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D3,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C3), Input!D3 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C3,Name2SID!D:D,0)))</f>
         <v>1155989565</v>
       </c>
       <c r="B3" s="1" t="str">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A3,Name2SID!A:A,0))</f>
         <v>Leonhard EULER</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>989565</v>
       </c>
       <c r="E3" s="1">
@@ -691,18 +694,18 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <f>IF(ISBLANK(Input!D4), Input!C4 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D4,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C4), Input!D4 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C4,Name2SID!D:D,0)))</f>
         <v>1155111111</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A4,Name2SID!A:A,0))</f>
         <v>Terence TAO</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3">
         <v>141566</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E4" s="1">
         <v>25</v>
@@ -713,14 +716,14 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <f>IF(ISBLANK(Input!D5), Input!C5 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D5,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C5), Input!D5 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C5,Name2SID!D:D,0)))</f>
         <v>1155565651</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A5,Name2SID!A:A,0))</f>
         <v>Bernhard RIEMANN</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="1">
@@ -732,14 +735,14 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <f>IF(ISBLANK(Input!D6), Input!C6 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D6,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C6), Input!D6 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C6,Name2SID!D:D,0)))</f>
         <v>1155123456</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A6,Name2SID!A:A,0))</f>
         <v>San ZHANG</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="1">
@@ -751,7 +754,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <f>IF(ISBLANK(Input!D7), Input!C7 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D7,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C7), Input!D7 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C7,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B7" s="1" t="e">
@@ -767,7 +770,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f>IF(ISBLANK(Input!D8), Input!C8 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D8,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C8), Input!D8 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C8,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B8" s="1" t="e">
@@ -777,27 +780,27 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f>IF(ISBLANK(Input!D9), Input!C9 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D9,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C9), Input!D9 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C9,Name2SID!D:D,0)))</f>
         <v>1155232565</v>
       </c>
       <c r="B9" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A9,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <f>IF(ISBLANK(Input!D10), Input!C10 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D10,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C10), Input!D10 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C10,Name2SID!D:D,0)))</f>
         <v>1155111111</v>
       </c>
       <c r="B10" s="1" t="str">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A10,Name2SID!A:A,0))</f>
         <v>Terence TAO</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="1">
@@ -809,7 +812,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <f>IF(ISBLANK(Input!D11), Input!C11 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D11,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C11), Input!D11 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C11,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B11" s="1" t="e">
@@ -819,14 +822,14 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <f>IF(ISBLANK(Input!D12), Input!C12 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D12,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C12), Input!D12 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C12,Name2SID!D:D,0)))</f>
         <v>1155123656</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A12,Name2SID!A:A,0))</f>
         <v>Wu WANG</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E12" s="1">
@@ -839,14 +842,14 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <f>IF(ISBLANK(Input!D13), Input!C13 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D13,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C13), Input!D13 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C13,Name2SID!D:D,0)))</f>
         <v>1155232898</v>
       </c>
       <c r="B13" s="1" t="str">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A13,Name2SID!A:A,0))</f>
         <v>Hello WORLD</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="1">
@@ -858,17 +861,26 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <f>IF(ISBLANK(Input!D14), Input!C14 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D14,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
-      </c>
-      <c r="B14" s="1" t="e">
+        <f>IF(ISBLANK(Input!C14), Input!D14 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C14,Name2SID!D:D,0)))</f>
+        <v>1155232898</v>
+      </c>
+      <c r="B14" s="1" t="str">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A14,Name2SID!A:A,0))</f>
-        <v>#N/A</v>
+        <v>Hello WORLD</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="1">
+        <v>232</v>
+      </c>
+      <c r="F14" s="1">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <f>IF(ISBLANK(Input!D15), Input!C15 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D15,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C15), Input!D15 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C15,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B15" s="1" t="e">
@@ -878,7 +890,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <f>IF(ISBLANK(Input!D16), Input!C16 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D16,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C16), Input!D16 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C16,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B16" s="1" t="e">
@@ -888,7 +900,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <f>IF(ISBLANK(Input!D17), Input!C17 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D17,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C17), Input!D17 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C17,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B17" s="1" t="e">
@@ -898,7 +910,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <f>IF(ISBLANK(Input!D18), Input!C18 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D18,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C18), Input!D18 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C18,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B18" s="1" t="e">
@@ -908,7 +920,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <f>IF(ISBLANK(Input!D19), Input!C19 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D19,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C19), Input!D19 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C19,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B19" s="1" t="e">
@@ -918,7 +930,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <f>IF(ISBLANK(Input!D20), Input!C20 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D20,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C20), Input!D20 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C20,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B20" s="1" t="e">
@@ -928,7 +940,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <f>IF(ISBLANK(Input!D21), Input!C21 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D21,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C21), Input!D21 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C21,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B21" s="1" t="e">
@@ -938,7 +950,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <f>IF(ISBLANK(Input!D22), Input!C22 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D22,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C22), Input!D22 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C22,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B22" s="1" t="e">
@@ -948,7 +960,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <f>IF(ISBLANK(Input!D23), Input!C23 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D23,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C23), Input!D23 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C23,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B23" s="1" t="e">
@@ -958,7 +970,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <f>IF(ISBLANK(Input!D24), Input!C24 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D24,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C24), Input!D24 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C24,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B24" s="1" t="e">
@@ -968,7 +980,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <f>IF(ISBLANK(Input!D25), Input!C25 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D25,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C25), Input!D25 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C25,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B25" s="1" t="e">
@@ -978,7 +990,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <f>IF(ISBLANK(Input!D26), Input!C26 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D26,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C26), Input!D26 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C26,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B26" s="1" t="e">
@@ -988,7 +1000,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <f>IF(ISBLANK(Input!D27), Input!C27 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D27,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C27), Input!D27 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C27,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B27" s="1" t="e">
@@ -998,7 +1010,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <f>IF(ISBLANK(Input!D28), Input!C28 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D28,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C28), Input!D28 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C28,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B28" s="1" t="e">
@@ -1008,7 +1020,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <f>IF(ISBLANK(Input!D29), Input!C29 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D29,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C29), Input!D29 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C29,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B29" s="1" t="e">
@@ -1018,7 +1030,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <f>IF(ISBLANK(Input!D30), Input!C30 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D30,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C30), Input!D30 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C30,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B30" s="1" t="e">
@@ -1028,7 +1040,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <f>IF(ISBLANK(Input!D31), Input!C31 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D31,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C31), Input!D31 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C31,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B31" s="1" t="e">
@@ -1038,7 +1050,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <f>IF(ISBLANK(Input!D32), Input!C32 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D32,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C32), Input!D32 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C32,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B32" s="1" t="e">
@@ -1048,7 +1060,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <f>IF(ISBLANK(Input!D33), Input!C33 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D33,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C33), Input!D33 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C33,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B33" s="1" t="e">
@@ -1058,7 +1070,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <f>IF(ISBLANK(Input!D34), Input!C34 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D34,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C34), Input!D34 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C34,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B34" s="1" t="e">
@@ -1068,7 +1080,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <f>IF(ISBLANK(Input!D35), Input!C35 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D35,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C35), Input!D35 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C35,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B35" s="1" t="e">
@@ -1078,7 +1090,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <f>IF(ISBLANK(Input!D36), Input!C36 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!D36,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C36), Input!D36 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C36,Name2SID!D:D,0)))</f>
         <v>1155000000</v>
       </c>
       <c r="B36" s="1" t="e">
@@ -1094,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1119,7 @@
     <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="6" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="26" width="9.140625" customWidth="1"/>
     <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1481,7 +1493,7 @@
       </c>
       <c r="B9" s="1">
         <f>COUNTIF(Input!A:A,Output!A9)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>Name2SID!B9</f>
@@ -1520,18 +1532,252 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+    </row>
   </sheetData>
   <autoFilter ref="B1:B7"/>
   <conditionalFormatting sqref="B2:B9">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B9">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1545,7 +1791,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,12 +1998,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E958">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="E2:E957">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1769,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,6 +2216,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037EA8EFF7603AD4589909F2D6CDAEF87" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1204792ee41e8d2f815be72486018407">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e3cef67-c514-4257-80f7-3488369f6876" xmlns:ns4="3ef59f0b-425e-41d0-9729-9f55f01e369c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d365b7dfa1eb6cee661573828196401b" ns3:_="" ns4:_="">
     <xsd:import namespace="8e3cef67-c514-4257-80f7-3488369f6876"/>
@@ -2192,22 +2453,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5333C76-115D-42A1-88EF-903D02FC6396}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3ef59f0b-425e-41d0-9729-9f55f01e369c"/>
+    <ds:schemaRef ds:uri="8e3cef67-c514-4257-80f7-3488369f6876"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77EE8607-BA45-45DE-BE65-B1415EAF701D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85B987F8-BB67-4BF3-87FF-552DF7D9BB4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2224,29 +2495,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77EE8607-BA45-45DE-BE65-B1415EAF701D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5333C76-115D-42A1-88EF-903D02FC6396}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3ef59f0b-425e-41d0-9729-9f55f01e369c"/>
-    <ds:schemaRef ds:uri="8e3cef67-c514-4257-80f7-3488369f6876"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
set default SID 11551*****
</commit_message>
<xml_diff>
--- a/TA/InputGrades.xlsx
+++ b/TA/InputGrades.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\toolkit\TA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zfeng/github/toolkit/TA/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15436AF1-D2B8-D245-97A4-48D9E8E8DD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -20,10 +21,21 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Output!$B$1:$B$7</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -143,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -517,26 +529,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CN36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="1" max="1" width="33.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="1" customWidth="1"/>
+    <col min="6" max="9" width="9.1640625" style="1"/>
     <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="str">
         <f>Name2SID!A1</f>
         <v>Student ID</v>
@@ -904,9 +916,9 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <f>IF(ISBLANK(Input!C2), Input!D2 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C2,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C2), Input!D2 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C2,Name2SID!D:D,0)))</f>
         <v>1155000001</v>
       </c>
       <c r="B2" s="1" t="str">
@@ -920,14 +932,14 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <f>IF(ISBLANK(Input!C3), Input!D3 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C3,Name2SID!D:D,0)))</f>
-        <v>1155989565</v>
-      </c>
-      <c r="B3" s="1" t="str">
+        <f>IF(ISBLANK(Input!C3), Input!D3 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C3,Name2SID!D:D,0)))</f>
+        <v>1156089565</v>
+      </c>
+      <c r="B3" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A3,Name2SID!A:A,0))</f>
-        <v>Leonhard EULER</v>
+        <v>#N/A</v>
       </c>
       <c r="D3" s="2">
         <v>989565</v>
@@ -939,9 +951,9 @@
         <v>-22</v>
       </c>
     </row>
-    <row r="4" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <f>IF(ISBLANK(Input!C4), Input!D4 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C4,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C4), Input!D4 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C4,Name2SID!D:D,0)))</f>
         <v>1155111111</v>
       </c>
       <c r="B4" s="1" t="str">
@@ -961,9 +973,9 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <f>IF(ISBLANK(Input!C5), Input!D5 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C5,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C5), Input!D5 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C5,Name2SID!D:D,0)))</f>
         <v>1155565651</v>
       </c>
       <c r="B5" s="1" t="str">
@@ -980,14 +992,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <f>IF(ISBLANK(Input!C6), Input!D6 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C6,Name2SID!D:D,0)))</f>
-        <v>1155123456</v>
-      </c>
-      <c r="B6" s="1" t="str">
+        <f>IF(ISBLANK(Input!C6), Input!D6 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C6,Name2SID!D:D,0)))</f>
+        <v>1155223456</v>
+      </c>
+      <c r="B6" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A6,Name2SID!A:A,0))</f>
-        <v>San ZHANG</v>
+        <v>#N/A</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -999,10 +1011,10 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <f>IF(ISBLANK(Input!C7), Input!D7 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C7,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C7), Input!D7 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C7,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B7" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A7,Name2SID!A:A,0))</f>
@@ -1015,20 +1027,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <f>IF(ISBLANK(Input!C8), Input!D8 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C8,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C8), Input!D8 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C8,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B8" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A8,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <f>IF(ISBLANK(Input!C9), Input!D9 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C9,Name2SID!D:D,0)))</f>
-        <v>1155232565</v>
+        <f>IF(ISBLANK(Input!C9), Input!D9 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C9,Name2SID!D:D,0)))</f>
+        <v>1155332565</v>
       </c>
       <c r="B9" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A9,Name2SID!A:A,0))</f>
@@ -1038,9 +1050,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <f>IF(ISBLANK(Input!C10), Input!D10 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C10,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C10), Input!D10 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C10,Name2SID!D:D,0)))</f>
         <v>1155111111</v>
       </c>
       <c r="B10" s="1" t="str">
@@ -1057,19 +1069,19 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <f>IF(ISBLANK(Input!C11), Input!D11 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C11,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C11), Input!D11 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C11,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B11" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A11,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <f>IF(ISBLANK(Input!C12), Input!D12 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C12,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C12), Input!D12 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C12,Name2SID!D:D,0)))</f>
         <v>1155123656</v>
       </c>
       <c r="B12" s="1" t="str">
@@ -1084,9 +1096,9 @@
       </c>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <f>IF(ISBLANK(Input!C13), Input!D13 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C13,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C13), Input!D13 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C13,Name2SID!D:D,0)))</f>
         <v>1155232898</v>
       </c>
       <c r="B13" s="1" t="str">
@@ -1103,9 +1115,9 @@
         <v>1.032</v>
       </c>
     </row>
-    <row r="14" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <f>IF(ISBLANK(Input!C14), Input!D14 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C14,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C14), Input!D14 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C14,Name2SID!D:D,0)))</f>
         <v>1155232898</v>
       </c>
       <c r="B14" s="1" t="str">
@@ -1116,9 +1128,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="e">
-        <f>IF(ISBLANK(Input!C15), Input!D15 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C15,Name2SID!D:D,0)))</f>
+        <f>IF(ISBLANK(Input!C15), Input!D15 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C15,Name2SID!D:D,0)))</f>
         <v>#N/A</v>
       </c>
       <c r="B15" s="1" t="e">
@@ -1129,210 +1141,210 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <f>IF(ISBLANK(Input!C16), Input!D16 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C16,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C16), Input!D16 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C16,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B16" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A16,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <f>IF(ISBLANK(Input!C17), Input!D17 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C17,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C17), Input!D17 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C17,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B17" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A17,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <f>IF(ISBLANK(Input!C18), Input!D18 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C18,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C18), Input!D18 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C18,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B18" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A18,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <f>IF(ISBLANK(Input!C19), Input!D19 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C19,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C19), Input!D19 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C19,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B19" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A19,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <f>IF(ISBLANK(Input!C20), Input!D20 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C20,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C20), Input!D20 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C20,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B20" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A20,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <f>IF(ISBLANK(Input!C21), Input!D21 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C21,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C21), Input!D21 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C21,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B21" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A21,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <f>IF(ISBLANK(Input!C22), Input!D22 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C22,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C22), Input!D22 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C22,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B22" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A22,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <f>IF(ISBLANK(Input!C23), Input!D23 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C23,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C23), Input!D23 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C23,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B23" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A23,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <f>IF(ISBLANK(Input!C24), Input!D24 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C24,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C24), Input!D24 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C24,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B24" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A24,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <f>IF(ISBLANK(Input!C25), Input!D25 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C25,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C25), Input!D25 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C25,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B25" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A25,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <f>IF(ISBLANK(Input!C26), Input!D26 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C26,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C26), Input!D26 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C26,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B26" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A26,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <f>IF(ISBLANK(Input!C27), Input!D27 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C27,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C27), Input!D27 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C27,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B27" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A27,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <f>IF(ISBLANK(Input!C28), Input!D28 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C28,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C28), Input!D28 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C28,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B28" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A28,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <f>IF(ISBLANK(Input!C29), Input!D29 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C29,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C29), Input!D29 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C29,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B29" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A29,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
-        <f>IF(ISBLANK(Input!C30), Input!D30 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C30,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C30), Input!D30 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C30,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B30" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A30,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
-        <f>IF(ISBLANK(Input!C31), Input!D31 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C31,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C31), Input!D31 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C31,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B31" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A31,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
-        <f>IF(ISBLANK(Input!C32), Input!D32 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C32,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C32), Input!D32 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C32,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B32" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A32,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
-        <f>IF(ISBLANK(Input!C33), Input!D33 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C33,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C33), Input!D33 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C33,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B33" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A33,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
-        <f>IF(ISBLANK(Input!C34), Input!D34 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C34,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C34), Input!D34 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C34,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B34" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A34,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
-        <f>IF(ISBLANK(Input!C35), Input!D35 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C35,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C35), Input!D35 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C35,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B35" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A35,Name2SID!A:A,0))</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
-        <f>IF(ISBLANK(Input!C36), Input!D36 + 1155000000, INDEX(Name2SID!A:A,MATCH(Input!C36,Name2SID!D:D,0)))</f>
-        <v>1155000000</v>
+        <f>IF(ISBLANK(Input!C36), Input!D36 + 1155100000, INDEX(Name2SID!A:A,MATCH(Input!C36,Name2SID!D:D,0)))</f>
+        <v>1155100000</v>
       </c>
       <c r="B36" s="1" t="e">
         <f>INDEX(Name2SID!D:D,MATCH(Input!A36,Name2SID!A:A,0))</f>
@@ -1346,25 +1358,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="8" width="12.42578125" style="1" customWidth="1"/>
-    <col min="9" max="25" width="9.140625" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="8" width="12.5" style="1" customWidth="1"/>
+    <col min="9" max="25" width="9.1640625" customWidth="1"/>
+    <col min="26" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
         <f>Name2SID!A1</f>
         <v>Student ID</v>
@@ -1404,7 +1416,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <f>Name2SID!A2</f>
         <v>1155000001</v>
@@ -1447,7 +1459,7 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f>Name2SID!A3</f>
         <v>1155111111</v>
@@ -1490,14 +1502,14 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f>Name2SID!A4</f>
         <v>1155123456</v>
       </c>
       <c r="B4" s="1">
         <f>COUNTIF(Input!A:A,Output!A4)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>Name2SID!B4</f>
@@ -1507,13 +1519,13 @@
         <f>Name2SID!C4</f>
         <v>San</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="1" t="e">
         <f>IF(ISBLANK(INDEX(Input!E:E,MATCH(Output!$A4,Input!$A:$A,0))), "", INDEX(Input!E:E,MATCH(Output!$A4,Input!$A:$A,0)))</f>
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
+        <v>#N/A</v>
+      </c>
+      <c r="F4" s="1" t="e">
         <f>IF(ISBLANK(INDEX(Input!F:F,MATCH(Output!$A4,Input!$A:$A,0))), "", INDEX(Input!F:F,MATCH(Output!$A4,Input!$A:$A,0)))</f>
-        <v>262</v>
+        <v>#N/A</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1533,7 +1545,7 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f>Name2SID!A5</f>
         <v>1155566202</v>
@@ -1576,14 +1588,14 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f>Name2SID!A6</f>
         <v>1155989565</v>
       </c>
       <c r="B6" s="1">
         <f>COUNTIF(Input!A:A,Output!A6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>Name2SID!B6</f>
@@ -1593,13 +1605,13 @@
         <f>Name2SID!C6</f>
         <v>Leonhard</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="1" t="e">
         <f>IF(ISBLANK(INDEX(Input!E:E,MATCH(Output!$A6,Input!$A:$A,0))), "", INDEX(Input!E:E,MATCH(Output!$A6,Input!$A:$A,0)))</f>
-        <v>99</v>
-      </c>
-      <c r="F6" s="1">
+        <v>#N/A</v>
+      </c>
+      <c r="F6" s="1" t="e">
         <f>IF(ISBLANK(INDEX(Input!F:F,MATCH(Output!$A6,Input!$A:$A,0))), "", INDEX(Input!F:F,MATCH(Output!$A6,Input!$A:$A,0)))</f>
-        <v>-22</v>
+        <v>#N/A</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1619,7 +1631,7 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f>Name2SID!A7</f>
         <v>1155565651</v>
@@ -1662,7 +1674,7 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f>Name2SID!A8</f>
         <v>1155123656</v>
@@ -1705,7 +1717,7 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f>Name2SID!A9</f>
         <v>1155232898</v>
@@ -1748,7 +1760,7 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -1764,7 +1776,7 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -1780,7 +1792,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -1796,7 +1808,7 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -1812,7 +1824,7 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -1828,7 +1840,7 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -1844,7 +1856,7 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -1860,7 +1872,7 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -1876,7 +1888,7 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -1892,7 +1904,7 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -1908,7 +1920,7 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -1924,7 +1936,7 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -1940,7 +1952,7 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -1956,7 +1968,7 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -1972,7 +1984,7 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -1988,7 +2000,7 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -2004,7 +2016,7 @@
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -2020,7 +2032,7 @@
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -2037,7 +2049,7 @@
       <c r="Y27" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B7"/>
+  <autoFilter ref="B1:B7" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="B2:B9">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>1</formula>
@@ -2057,23 +2069,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="30" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
         <f>RawList!$C$1</f>
         <v>Student ID</v>
@@ -2093,7 +2105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <f>RawList!C2</f>
         <v>1155000001</v>
@@ -2115,7 +2127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f>RawList!C3</f>
         <v>1155111111</v>
@@ -2137,7 +2149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f>RawList!C4</f>
         <v>1155123456</v>
@@ -2159,7 +2171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f>RawList!C5</f>
         <v>1155566202</v>
@@ -2181,7 +2193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f>RawList!C6</f>
         <v>1155989565</v>
@@ -2203,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f>RawList!C7</f>
         <v>1155565651</v>
@@ -2225,7 +2237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f>RawList!C8</f>
         <v>1155123656</v>
@@ -2247,7 +2259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f>RawList!C9</f>
         <v>1155232898</v>
@@ -2285,22 +2297,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="30" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="31.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2311,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -2322,7 +2335,7 @@
         <v>1155000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -2333,7 +2346,7 @@
         <v>1155111111</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -2344,7 +2357,7 @@
         <v>1155123456</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -2355,7 +2368,7 @@
         <v>1155566202</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -2366,7 +2379,7 @@
         <v>1155989565</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -2377,7 +2390,7 @@
         <v>1155565651</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -2388,7 +2401,7 @@
         <v>1155123656</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -2405,21 +2418,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037EA8EFF7603AD4589909F2D6CDAEF87" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1204792ee41e8d2f815be72486018407">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8e3cef67-c514-4257-80f7-3488369f6876" xmlns:ns4="3ef59f0b-425e-41d0-9729-9f55f01e369c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d365b7dfa1eb6cee661573828196401b" ns3:_="" ns4:_="">
     <xsd:import namespace="8e3cef67-c514-4257-80f7-3488369f6876"/>
@@ -2642,32 +2640,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5333C76-115D-42A1-88EF-903D02FC6396}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3ef59f0b-425e-41d0-9729-9f55f01e369c"/>
-    <ds:schemaRef ds:uri="8e3cef67-c514-4257-80f7-3488369f6876"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77EE8607-BA45-45DE-BE65-B1415EAF701D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85B987F8-BB67-4BF3-87FF-552DF7D9BB4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2684,4 +2672,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77EE8607-BA45-45DE-BE65-B1415EAF701D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5333C76-115D-42A1-88EF-903D02FC6396}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3ef59f0b-425e-41d0-9729-9f55f01e369c"/>
+    <ds:schemaRef ds:uri="8e3cef67-c514-4257-80f7-3488369f6876"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>